<commit_message>
add pass test mark and add ranking function
</commit_message>
<xml_diff>
--- a/test/1. 各院彙整資料/傳播學院.xlsx
+++ b/test/1. 各院彙整資料/傳播學院.xlsx
@@ -5,34 +5,34 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\學評組工讀生\應數碩三_陳慎逸\程式學習\Index-Evaluation-Analysis-Report\test\1. 各院彙整資料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\學評組工讀生\應數碩三_陳慎逸\3. Index-Evaluation-Analysis-Report\test\1. 各院彙整資料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B8DF31-2B3E-4ABA-8ADD-646B8B48B45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8FBA2F-671D-4B29-A31D-6CF99A5B83F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{7724BB71-FDD3-4610-87B4-A17FEA766B3C}"/>
+    <workbookView xWindow="1950" yWindow="600" windowWidth="17595" windowHeight="15600" firstSheet="4" activeTab="7" xr2:uid="{7724BB71-FDD3-4610-87B4-A17FEA766B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="小結" sheetId="1" r:id="rId1"/>
-    <sheet name="1.1.1.1 學士班繁星推薦入學錄取率" sheetId="2" r:id="rId2"/>
-    <sheet name="1.1.3.4 博士班招收國內重點大學畢業生比率" sheetId="3" r:id="rId3"/>
-    <sheet name="1.4.1.1 學士班獲獎助學金平均金額" sheetId="4" r:id="rId4"/>
-    <sheet name="1.7.1.4 碩士班平均修業年限" sheetId="5" r:id="rId5"/>
-    <sheet name="2.1.1.2 平均碩博士班修課學生人數" sheetId="6" r:id="rId6"/>
-    <sheet name="2.3.1.2 各系所教師兼任本校二級學術行政主管人次" sheetId="7" r:id="rId7"/>
-    <sheet name="3.2.1.1 舉辦國際學術研討會數" sheetId="8" r:id="rId8"/>
+    <sheet name="1.1.1.1 學士班繁星推薦入學錄取率" sheetId="9" r:id="rId2"/>
+    <sheet name="1.1.3.4 博士班招收國內重點大學畢業生比率" sheetId="10" r:id="rId3"/>
+    <sheet name="1.4.1.1 學士班獲獎助學金平均金額" sheetId="11" r:id="rId4"/>
+    <sheet name="1.7.1.4 碩士班平均修業年限" sheetId="12" r:id="rId5"/>
+    <sheet name="2.1.1.2 平均碩博士班修課學生人數" sheetId="13" r:id="rId6"/>
+    <sheet name="2.3.1.2 各系所教師兼任本校二級學術行政主管人次" sheetId="14" r:id="rId7"/>
+    <sheet name="3.2.1.1 舉辦國際學術研討會數" sheetId="15" r:id="rId8"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1.1.1.1 學士班繁星推薦入學錄取率'!$A$1:$G$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'1.1.3.4 博士班招收國內重點大學畢業生比率'!$A$1:$G$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'1.4.1.1 學士班獲獎助學金平均金額'!$A$1:$G$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'1.7.1.4 碩士班平均修業年限'!$A$1:$G$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2.1.1.2 平均碩博士班修課學生人數'!$A$1:$G$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$A$1:$G$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'3.2.1.1 舉辦國際學術研討會數'!$A$1:$G$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1.1.1.1 學士班繁星推薦入學錄取率'!$A$1:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'1.1.3.4 博士班招收國內重點大學畢業生比率'!$A$1:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'1.4.1.1 學士班獲獎助學金平均金額'!$A$1:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'1.7.1.4 碩士班平均修業年限'!$A$1:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2.1.1.2 平均碩博士班修課學生人數'!$A$1:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$A$1:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'3.2.1.1 舉辦國際學術研討會數'!$A$1:$G$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="37">
   <si>
     <t>傳播學院</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>400 傳播學院（院加總 / 院均值）</t>
-  </si>
-  <si>
-    <t>400 傳播學院</t>
   </si>
   <si>
     <t>401 新聞學系</t>
@@ -491,40 +488,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$B$2:$B$12</c:f>
+              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -532,14 +526,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$F$2:$F$12</c:f>
+              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -547,7 +541,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6D29-4777-B20E-7012A515CB47}"/>
+              <c16:uniqueId val="{00000000-F830-49F6-90F4-4FE5F133EC39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -582,40 +576,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$B$2:$B$12</c:f>
+              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -623,14 +614,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$E$2:$E$12</c:f>
+              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.03</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -638,7 +629,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6D29-4777-B20E-7012A515CB47}"/>
+              <c16:uniqueId val="{00000001-F830-49F6-90F4-4FE5F133EC39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -673,40 +664,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$B$2:$B$12</c:f>
+              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -714,14 +702,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$D$2:$D$12</c:f>
+              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -729,7 +717,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6D29-4777-B20E-7012A515CB47}"/>
+              <c16:uniqueId val="{00000002-F830-49F6-90F4-4FE5F133EC39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -840,7 +828,7 @@
                   </c15:spPr>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-6D29-4777-B20E-7012A515CB47}"/>
+                  <c16:uniqueId val="{00000003-F830-49F6-90F4-4FE5F133EC39}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -912,40 +900,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$B$2:$B$12</c:f>
+              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -953,14 +938,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$C$2:$C$12</c:f>
+              <c:f>'1.1.1.1 學士班繁星推薦入學錄取率'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
@@ -969,7 +954,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-6D29-4777-B20E-7012A515CB47}"/>
+              <c16:uniqueId val="{00000004-F830-49F6-90F4-4FE5F133EC39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1250,40 +1235,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$B$2:$B$12</c:f>
+              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -1291,14 +1273,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$F$2:$F$12</c:f>
+              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1306,7 +1288,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E009-4404-A320-7EB3C1D04042}"/>
+              <c16:uniqueId val="{00000000-BC18-4660-9286-61AC8616BCF9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1341,40 +1323,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$B$2:$B$12</c:f>
+              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -1382,14 +1361,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$E$2:$E$12</c:f>
+              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.03</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -1397,7 +1376,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E009-4404-A320-7EB3C1D04042}"/>
+              <c16:uniqueId val="{00000001-BC18-4660-9286-61AC8616BCF9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1432,40 +1411,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$B$2:$B$12</c:f>
+              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -1473,14 +1449,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$D$2:$D$12</c:f>
+              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -1488,7 +1464,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E009-4404-A320-7EB3C1D04042}"/>
+              <c16:uniqueId val="{00000002-BC18-4660-9286-61AC8616BCF9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1599,7 +1575,7 @@
                   </c15:spPr>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-E009-4404-A320-7EB3C1D04042}"/>
+                  <c16:uniqueId val="{00000003-BC18-4660-9286-61AC8616BCF9}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1671,40 +1647,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$B$2:$B$12</c:f>
+              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -1712,14 +1685,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$C$2:$C$12</c:f>
+              <c:f>'1.1.3.4 博士班招收國內重點大學畢業生比率'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
@@ -1728,7 +1701,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-E009-4404-A320-7EB3C1D04042}"/>
+              <c16:uniqueId val="{00000004-BC18-4660-9286-61AC8616BCF9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2009,40 +1982,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$B$2:$B$12</c:f>
+              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -2050,14 +2020,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$F$2:$F$12</c:f>
+              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -2065,7 +2035,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-82F8-4FEC-83B5-0D2D2B608BAA}"/>
+              <c16:uniqueId val="{00000000-75A7-4DF1-9B6F-2A8B75A0A4C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2100,40 +2070,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$B$2:$B$12</c:f>
+              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -2141,14 +2108,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$E$2:$E$12</c:f>
+              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.03</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -2156,7 +2123,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-82F8-4FEC-83B5-0D2D2B608BAA}"/>
+              <c16:uniqueId val="{00000001-75A7-4DF1-9B6F-2A8B75A0A4C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2191,40 +2158,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$B$2:$B$12</c:f>
+              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -2232,14 +2196,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$D$2:$D$12</c:f>
+              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -2247,7 +2211,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-82F8-4FEC-83B5-0D2D2B608BAA}"/>
+              <c16:uniqueId val="{00000002-75A7-4DF1-9B6F-2A8B75A0A4C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2358,7 +2322,7 @@
                   </c15:spPr>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-82F8-4FEC-83B5-0D2D2B608BAA}"/>
+                  <c16:uniqueId val="{00000003-75A7-4DF1-9B6F-2A8B75A0A4C3}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2430,40 +2394,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$B$2:$B$12</c:f>
+              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -2471,14 +2432,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$C$2:$C$12</c:f>
+              <c:f>'1.4.1.1 學士班獲獎助學金平均金額'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
@@ -2487,7 +2448,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-82F8-4FEC-83B5-0D2D2B608BAA}"/>
+              <c16:uniqueId val="{00000004-75A7-4DF1-9B6F-2A8B75A0A4C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2768,40 +2729,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.7.1.4 碩士班平均修業年限'!$B$2:$B$12</c:f>
+              <c:f>'1.7.1.4 碩士班平均修業年限'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -2809,14 +2767,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.7.1.4 碩士班平均修業年限'!$F$2:$F$12</c:f>
+              <c:f>'1.7.1.4 碩士班平均修業年限'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -2824,7 +2782,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-41CE-4342-BCED-8361A7F71FEA}"/>
+              <c16:uniqueId val="{00000000-2164-4CD4-9B34-FDCDCFEB907C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2859,40 +2817,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.7.1.4 碩士班平均修業年限'!$B$2:$B$12</c:f>
+              <c:f>'1.7.1.4 碩士班平均修業年限'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -2900,14 +2855,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.7.1.4 碩士班平均修業年限'!$E$2:$E$12</c:f>
+              <c:f>'1.7.1.4 碩士班平均修業年限'!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.03</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -2915,7 +2870,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-41CE-4342-BCED-8361A7F71FEA}"/>
+              <c16:uniqueId val="{00000001-2164-4CD4-9B34-FDCDCFEB907C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2950,40 +2905,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.7.1.4 碩士班平均修業年限'!$B$2:$B$12</c:f>
+              <c:f>'1.7.1.4 碩士班平均修業年限'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -2991,14 +2943,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.7.1.4 碩士班平均修業年限'!$D$2:$D$12</c:f>
+              <c:f>'1.7.1.4 碩士班平均修業年限'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -3006,7 +2958,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-41CE-4342-BCED-8361A7F71FEA}"/>
+              <c16:uniqueId val="{00000002-2164-4CD4-9B34-FDCDCFEB907C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3117,7 +3069,7 @@
                   </c15:spPr>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-41CE-4342-BCED-8361A7F71FEA}"/>
+                  <c16:uniqueId val="{00000003-2164-4CD4-9B34-FDCDCFEB907C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3189,40 +3141,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'1.7.1.4 碩士班平均修業年限'!$B$2:$B$12</c:f>
+              <c:f>'1.7.1.4 碩士班平均修業年限'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -3230,14 +3179,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1.7.1.4 碩士班平均修業年限'!$C$2:$C$12</c:f>
+              <c:f>'1.7.1.4 碩士班平均修業年限'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
@@ -3246,7 +3195,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-41CE-4342-BCED-8361A7F71FEA}"/>
+              <c16:uniqueId val="{00000004-2164-4CD4-9B34-FDCDCFEB907C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3527,40 +3476,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$B$2:$B$12</c:f>
+              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -3568,14 +3514,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$F$2:$F$12</c:f>
+              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -3583,7 +3529,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-728B-451F-A1DF-45EAD17D48FC}"/>
+              <c16:uniqueId val="{00000000-F24A-4CEA-A6B6-EDAAFFEABB71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3618,40 +3564,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$B$2:$B$12</c:f>
+              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -3659,14 +3602,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$E$2:$E$12</c:f>
+              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.03</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -3674,7 +3617,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-728B-451F-A1DF-45EAD17D48FC}"/>
+              <c16:uniqueId val="{00000001-F24A-4CEA-A6B6-EDAAFFEABB71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3709,40 +3652,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$B$2:$B$12</c:f>
+              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -3750,14 +3690,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$D$2:$D$12</c:f>
+              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -3765,7 +3705,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-728B-451F-A1DF-45EAD17D48FC}"/>
+              <c16:uniqueId val="{00000002-F24A-4CEA-A6B6-EDAAFFEABB71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3876,7 +3816,7 @@
                   </c15:spPr>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-728B-451F-A1DF-45EAD17D48FC}"/>
+                  <c16:uniqueId val="{00000003-F24A-4CEA-A6B6-EDAAFFEABB71}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3948,40 +3888,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$B$2:$B$12</c:f>
+              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院均值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -3989,14 +3926,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$C$2:$C$12</c:f>
+              <c:f>'2.1.1.2 平均碩博士班修課學生人數'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
@@ -4005,7 +3942,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-728B-451F-A1DF-45EAD17D48FC}"/>
+              <c16:uniqueId val="{00000004-F24A-4CEA-A6B6-EDAAFFEABB71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4286,40 +4223,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$B$2:$B$12</c:f>
+              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院加總</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -4327,14 +4261,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$F$2:$F$12</c:f>
+              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -4342,7 +4276,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CF5D-4351-B8E9-AC131A584C0E}"/>
+              <c16:uniqueId val="{00000000-C703-4199-8789-BDAA4D8D2F19}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4377,40 +4311,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$B$2:$B$12</c:f>
+              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院加總</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -4418,14 +4349,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$E$2:$E$12</c:f>
+              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.03</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -4433,7 +4364,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CF5D-4351-B8E9-AC131A584C0E}"/>
+              <c16:uniqueId val="{00000001-C703-4199-8789-BDAA4D8D2F19}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4468,40 +4399,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$B$2:$B$12</c:f>
+              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院加總</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -4509,14 +4437,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$D$2:$D$12</c:f>
+              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -4524,7 +4452,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-CF5D-4351-B8E9-AC131A584C0E}"/>
+              <c16:uniqueId val="{00000002-C703-4199-8789-BDAA4D8D2F19}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4635,7 +4563,7 @@
                   </c15:spPr>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-CF5D-4351-B8E9-AC131A584C0E}"/>
+                  <c16:uniqueId val="{00000003-C703-4199-8789-BDAA4D8D2F19}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -4707,40 +4635,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$B$2:$B$12</c:f>
+              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院加總</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -4748,14 +4673,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$C$2:$C$12</c:f>
+              <c:f>'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
@@ -4764,7 +4689,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-CF5D-4351-B8E9-AC131A584C0E}"/>
+              <c16:uniqueId val="{00000004-C703-4199-8789-BDAA4D8D2F19}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5045,40 +4970,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$B$2:$B$12</c:f>
+              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院加總</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -5086,14 +5008,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$F$2:$F$12</c:f>
+              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -5101,7 +5023,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D4A1-46E8-8B07-2AC5DD1E4B69}"/>
+              <c16:uniqueId val="{00000000-F7D1-408B-A631-ECA9E881ECE5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5136,40 +5058,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$B$2:$B$12</c:f>
+              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院加總</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -5177,14 +5096,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$E$2:$E$12</c:f>
+              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.03</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -5192,7 +5111,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D4A1-46E8-8B07-2AC5DD1E4B69}"/>
+              <c16:uniqueId val="{00000001-F7D1-408B-A631-ECA9E881ECE5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5227,40 +5146,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$B$2:$B$12</c:f>
+              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院加總</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -5268,14 +5184,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$D$2:$D$12</c:f>
+              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -5283,7 +5199,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D4A1-46E8-8B07-2AC5DD1E4B69}"/>
+              <c16:uniqueId val="{00000002-F7D1-408B-A631-ECA9E881ECE5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5394,7 +5310,7 @@
                   </c15:spPr>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-D4A1-46E8-8B07-2AC5DD1E4B69}"/>
+                  <c16:uniqueId val="{00000003-F7D1-408B-A631-ECA9E881ECE5}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -5466,40 +5382,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$B$2:$B$12</c:f>
+              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>院加總</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳播學院</c:v>
+                  <c:v>新聞系</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>新聞系</c:v>
+                  <c:v>廣告系</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>廣告系</c:v>
+                  <c:v>廣電系</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>廣電系</c:v>
+                  <c:v>不分系</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>不分系</c:v>
+                  <c:v>國傳碩</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>國傳碩</c:v>
+                  <c:v>傳碩在</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>傳碩在</c:v>
+                  <c:v>數位碩</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>數位碩</c:v>
+                  <c:v>傳播博</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>傳播博</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>傳播碩</c:v>
                 </c:pt>
               </c:strCache>
@@ -5507,14 +5420,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$C$2:$C$12</c:f>
+              <c:f>'3.2.1.1 舉辦國際學術研討會數'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00;"—";"—"</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
@@ -5523,7 +5436,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D4A1-46E8-8B07-2AC5DD1E4B69}"/>
+              <c16:uniqueId val="{00000004-F7D1-408B-A631-ECA9E881ECE5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5752,7 +5665,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86AF0653-04BA-4B0E-8030-32B40CC10A54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F390ED48-4125-401A-B95F-05ECF9913441}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5785,7 +5698,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBA2B2E2-FFD7-407D-9556-217DD9B6A721}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BE7E5BA-D1CF-48C8-B75A-7F7E39B76ED4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5818,7 +5731,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E31C1437-ADB4-49C0-9958-C67A3D28CA90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89B7EEE6-81C2-4A73-BF01-CAB75A8B016B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5851,7 +5764,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B63E3DB3-55CD-4C2D-9572-428905EF9B0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90E6EAB8-8B4B-48B0-AA3C-BA688033EF07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5884,7 +5797,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7025AFFB-7D4E-4CC8-AE2A-573DF5118590}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3C00CFE-4D04-46A0-A8A3-0A50DA016398}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5917,7 +5830,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DC8C166-570E-4ECA-BEEF-6057D30986E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03894431-3000-4B13-B57A-DC73ED2B6821}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5950,7 +5863,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD02BC5E-90ED-49D4-A82F-727436FDEB71}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DE5C252-66F6-4CB2-B940-2B44B3BEDA78}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6000,7 +5913,7 @@
         </row>
         <row r="2">
           <cell r="B2" t="str">
-            <v>院均值</v>
+            <v>科系1</v>
           </cell>
           <cell r="C2">
             <v>0.06</v>
@@ -6017,7 +5930,7 @@
         </row>
         <row r="3">
           <cell r="B3" t="str">
-            <v>測試二</v>
+            <v>院均值</v>
           </cell>
           <cell r="C3">
             <v>0.05</v>
@@ -6418,25 +6331,25 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" location="'1.1.1.1 學士班繁星推薦入學錄取率'!A1" display="1.1.1.1 學士班繁星推薦入學錄取率" xr:uid="{21116269-1533-4454-A12B-2DB4B45513C8}"/>
-    <hyperlink ref="A3" location="'1.1.3.4 博士班招收國內重點大學畢業生比率'!A1" display="1.1.3.4 博士班招收國內重點大學畢業生比率" xr:uid="{B182A84D-D276-4711-AEC3-7AE0E1E15402}"/>
-    <hyperlink ref="A4" location="'1.4.1.1 學士班獲獎助學金平均金額'!A1" display="1.4.1.1 學士班獲獎助學金平均金額" xr:uid="{9B996E48-A8E3-4135-9198-77EA87474C0A}"/>
-    <hyperlink ref="A5" location="'1.7.1.4 碩士班平均修業年限'!A1" display="1.7.1.4 碩士班平均修業年限" xr:uid="{E31069D7-F273-44F2-9999-6D45C64FAA25}"/>
-    <hyperlink ref="A6" location="'2.1.1.2 平均碩博士班修課學生人數'!A1" display="2.1.1.2 平均碩博士班修課學生人數" xr:uid="{42BED922-B938-41CA-8FB7-6647C34B71E8}"/>
-    <hyperlink ref="A7" location="'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!A1" display="2.3.1.2 各系所教師兼任本校二級學術行政主管人次" xr:uid="{1A36965B-0551-41EB-8607-1817995F4087}"/>
-    <hyperlink ref="A8" location="'3.2.1.1 舉辦國際學術研討會數'!A1" display="3.2.1.1 舉辦國際學術研討會數" xr:uid="{1768AD99-7144-4993-BB53-1AF019782044}"/>
+    <hyperlink ref="A2" location="'1.1.1.1 學士班繁星推薦入學錄取率'!A1" display="1.1.1.1 學士班繁星推薦入學錄取率" xr:uid="{7C416EE3-A9A3-4AB6-825C-CDEFFE237134}"/>
+    <hyperlink ref="A3" location="'1.1.3.4 博士班招收國內重點大學畢業生比率'!A1" display="1.1.3.4 博士班招收國內重點大學畢業生比率" xr:uid="{08DE8C19-E887-4007-9DCA-0F444D1A1801}"/>
+    <hyperlink ref="A4" location="'1.4.1.1 學士班獲獎助學金平均金額'!A1" display="1.4.1.1 學士班獲獎助學金平均金額" xr:uid="{5CFB042C-8E2D-4582-B5E5-70992C7264D0}"/>
+    <hyperlink ref="A5" location="'1.7.1.4 碩士班平均修業年限'!A1" display="1.7.1.4 碩士班平均修業年限" xr:uid="{A6B1F25A-D66F-47DA-9503-791AB10D3DAD}"/>
+    <hyperlink ref="A6" location="'2.1.1.2 平均碩博士班修課學生人數'!A1" display="2.1.1.2 平均碩博士班修課學生人數" xr:uid="{7A4A694F-5FB0-4CD5-A83F-5F1E15E377B9}"/>
+    <hyperlink ref="A7" location="'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!A1" display="2.3.1.2 各系所教師兼任本校二級學術行政主管人次" xr:uid="{30E87CB4-A421-4787-A921-9D4A50418385}"/>
+    <hyperlink ref="A8" location="'3.2.1.1 舉辦國際學術研討會數'!A1" display="3.2.1.1 舉辦國際學術研討會數" xr:uid="{251C1C7E-7D1B-42E7-9DF2-4110FAE78D9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D621056-BFBD-4143-8E5D-B7E57815FAC2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA12EA6-A2C9-45E4-830C-3D1588E70260}">
   <sheetPr codeName="工作表2"/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6491,16 +6404,14 @@
       <c r="F2" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G2" s="9">
-        <v>999</v>
-      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -6513,7 +6424,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -6526,7 +6437,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -6539,7 +6450,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -6552,7 +6463,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -6565,7 +6476,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -6578,7 +6489,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -6591,7 +6502,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -6604,39 +6515,28 @@
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="C11" s="10">
         <v>0.05</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D11" s="10">
         <v>0.04</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E11" s="10">
         <v>0.01</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F11" s="10">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G11" s="9">
+        <v>999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-      <sortCondition descending="1" ref="G1:G12"/>
+  <autoFilter ref="A1:G11" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+      <sortCondition descending="1" ref="G1:G11"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6647,12 +6547,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FC7652-46D6-4BDB-9934-892C32322BBB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB515DC-8E0E-4F56-B0AC-434F415FEDB8}">
   <sheetPr codeName="工作表3"/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6707,16 +6607,14 @@
       <c r="F2" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G2" s="9">
-        <v>999</v>
-      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -6729,7 +6627,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -6742,7 +6640,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -6755,7 +6653,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -6768,7 +6666,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -6781,7 +6679,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -6794,7 +6692,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -6807,7 +6705,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -6820,39 +6718,28 @@
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="C11" s="10">
         <v>0.05</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D11" s="10">
         <v>0.04</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E11" s="10">
         <v>0.01</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F11" s="10">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G11" s="9">
+        <v>999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-      <sortCondition descending="1" ref="G1:G12"/>
+  <autoFilter ref="A1:G11" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+      <sortCondition descending="1" ref="G1:G11"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6863,12 +6750,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901AD3D1-22A9-4E3B-AAA7-C3BDEDD6A198}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231E3366-F74F-4C47-A6EE-0AF453A1CB23}">
   <sheetPr codeName="工作表4"/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6923,16 +6810,14 @@
       <c r="F2" s="11">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G2" s="9">
-        <v>999</v>
-      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -6945,7 +6830,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -6958,7 +6843,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -6971,7 +6856,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -6984,7 +6869,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -6997,7 +6882,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -7010,7 +6895,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -7023,7 +6908,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -7036,39 +6921,28 @@
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="11">
+      <c r="C11" s="11">
         <v>0.05</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D11" s="11">
         <v>0.04</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E11" s="11">
         <v>0.01</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F11" s="11">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G11" s="9">
+        <v>999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-      <sortCondition descending="1" ref="G1:G12"/>
+  <autoFilter ref="A1:G11" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+      <sortCondition descending="1" ref="G1:G11"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7079,12 +6953,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8FE0F1-7D2A-495D-9E1E-743AFB1E51A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B0A1D9-A6D6-42CE-A6F8-4E3FDE2A91FF}">
   <sheetPr codeName="工作表5"/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7139,16 +7013,14 @@
       <c r="F2" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G2" s="9">
-        <v>999</v>
-      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -7161,7 +7033,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -7174,7 +7046,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -7187,7 +7059,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -7200,7 +7072,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -7213,7 +7085,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -7226,7 +7098,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -7239,7 +7111,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -7252,39 +7124,28 @@
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="C11" s="12">
         <v>0.05</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D11" s="12">
         <v>0.04</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E11" s="12">
         <v>0.01</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F11" s="12">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G11" s="9">
+        <v>999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-      <sortCondition descending="1" ref="G1:G12"/>
+  <autoFilter ref="A1:G11" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+      <sortCondition descending="1" ref="G1:G11"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7295,12 +7156,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A5AE3D-77A4-464A-9F84-F21D122CAF04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13014F3F-0EA3-4EAF-9189-E2372496D067}">
   <sheetPr codeName="工作表6"/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7355,16 +7216,14 @@
       <c r="F2" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G2" s="9">
-        <v>999</v>
-      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -7377,7 +7236,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -7390,7 +7249,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -7403,7 +7262,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -7416,7 +7275,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -7429,7 +7288,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -7442,7 +7301,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -7455,7 +7314,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -7468,39 +7327,28 @@
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="C11" s="12">
         <v>0.05</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D11" s="12">
         <v>0.04</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E11" s="12">
         <v>0.01</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F11" s="12">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G11" s="9">
+        <v>999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-      <sortCondition descending="1" ref="G1:G12"/>
+  <autoFilter ref="A1:G11" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+      <sortCondition descending="1" ref="G1:G11"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7511,12 +7359,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B1B22E-B3A0-4345-8207-332E3B48BF3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DCC311-C650-4A5E-98EE-AC66C88471C9}">
   <sheetPr codeName="工作表7"/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7557,7 +7405,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="12">
         <v>0.06</v>
@@ -7571,16 +7419,14 @@
       <c r="F2" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G2" s="9">
-        <v>999</v>
-      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -7593,7 +7439,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -7606,7 +7452,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -7619,7 +7465,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -7632,7 +7478,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -7645,7 +7491,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -7658,7 +7504,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -7671,7 +7517,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -7684,39 +7530,28 @@
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="C11" s="12">
         <v>0.05</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D11" s="12">
         <v>0.04</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E11" s="12">
         <v>0.01</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F11" s="12">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G11" s="9">
+        <v>999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-      <sortCondition descending="1" ref="G1:G12"/>
+  <autoFilter ref="A1:G11" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+      <sortCondition descending="1" ref="G1:G11"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7727,12 +7562,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BAEEA4-0034-4B30-87BF-AC3DF9E3E328}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C583F2-9B22-435C-A681-101AAED6A23E}">
   <sheetPr codeName="工作表8"/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7773,7 +7608,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="12">
         <v>0.06</v>
@@ -7787,16 +7622,14 @@
       <c r="F2" s="12">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G2" s="9">
-        <v>999</v>
-      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -7809,7 +7642,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -7822,7 +7655,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -7835,7 +7668,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -7848,7 +7681,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -7861,7 +7694,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -7874,7 +7707,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -7887,7 +7720,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -7900,39 +7733,28 @@
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="C11" s="12">
         <v>0.05</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D11" s="12">
         <v>0.04</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E11" s="12">
         <v>0.01</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F11" s="12">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G11" s="9">
+        <v>999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-      <sortCondition descending="1" ref="G1:G12"/>
+  <autoFilter ref="A1:G11" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+      <sortCondition descending="1" ref="G1:G11"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add import modules remove unpublish pack
</commit_message>
<xml_diff>
--- a/test/1. 各院彙整資料/傳播學院.xlsx
+++ b/test/1. 各院彙整資料/傳播學院.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\學評組工讀生\應數碩三_陳慎逸\3. Index-Evaluation-Analysis-Report\test\1. 各院彙整資料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3555838-E6F1-4A70-8AC9-52A916838E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EF2F9D-699A-4B09-81FF-DD3B1ECDACB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{2F48443A-10B0-4271-8EB6-1234EEF64542}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="14580" windowHeight="10230" firstSheet="5" activeTab="7" xr2:uid="{2F48443A-10B0-4271-8EB6-1234EEF64542}"/>
   </bookViews>
   <sheets>
     <sheet name="小結" sheetId="1" r:id="rId1"/>
-    <sheet name="1.1.1.1 學士班繁星推薦入學錄取率" sheetId="93" r:id="rId2"/>
-    <sheet name="1.1.3.4 博士班招收國內重點大學畢業生比率" sheetId="94" r:id="rId3"/>
-    <sheet name="1.4.1.1 學士班獲獎助學金平均金額" sheetId="95" r:id="rId4"/>
-    <sheet name="1.7.1.4 碩士班平均修業年限" sheetId="96" r:id="rId5"/>
-    <sheet name="2.1.1.2 平均碩博士班修課學生人數" sheetId="97" r:id="rId6"/>
-    <sheet name="2.3.1.2 各系所教師兼任本校二級學術行政主管人次" sheetId="98" r:id="rId7"/>
-    <sheet name="3.2.1.1 舉辦國際學術研討會數" sheetId="99" r:id="rId8"/>
+    <sheet name="1.1.1.1 學士班繁星推薦入學錄取率" sheetId="100" r:id="rId2"/>
+    <sheet name="1.1.3.4 博士班招收國內重點大學畢業生比率" sheetId="101" r:id="rId3"/>
+    <sheet name="1.4.1.1 學士班獲獎助學金平均金額" sheetId="102" r:id="rId4"/>
+    <sheet name="1.7.1.4 碩士班平均修業年限" sheetId="103" r:id="rId5"/>
+    <sheet name="2.1.1.2 平均碩博士班修課學生人數" sheetId="104" r:id="rId6"/>
+    <sheet name="2.3.1.2 各系所教師兼任本校二級學術行政主管人次" sheetId="105" r:id="rId7"/>
+    <sheet name="3.2.1.1 舉辦國際學術研討會數" sheetId="106" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1.1.1.1 學士班繁星推薦入學錄取率'!$A$1:$G$11</definedName>
@@ -200,38 +200,31 @@
     <t>小結 3</t>
   </si>
   <si>
-    <t>小結 2</t>
+    <t>平均 1</t>
   </si>
   <si>
-    <t>小結 1</t>
+    <t>平均 2</t>
   </si>
   <si>
     <t>—</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>院三年均值為20.3%，低於（或等於）院三年均值者計有1個系，為不分系20.3%。</t>
   </si>
   <si>
     <t>院三年均值為47.62%，高於（或等於）院三年均值者計有1個系，為傳播博47.62%。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>院三年均值為42,888，高於院三年均值者計有1個系，為新聞系53,773。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>院三年均值為3.52，低於院三年均值者計有3個系，為數位碩2.56、國傳碩3.02、傳播碩3.48。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>院三年均值為15.4，無高於（或等於）院三年均值者。</t>
   </si>
   <si>
     <t>無資料。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>院三年均值為20.3%，低於（或等於）院三年均值者計有1個系，為不分系20.3%。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>院三年均值為15.4，無高於（或等於）院三年均值者。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -240,10 +233,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="177" formatCode="&quot;—&quot;"/>
-    <numFmt numFmtId="178" formatCode="#,##0;\-#,###;0"/>
-    <numFmt numFmtId="179" formatCode="###.##%;\-###.##%;0%"/>
-    <numFmt numFmtId="180" formatCode="###%;###%;0%"/>
+    <numFmt numFmtId="177" formatCode="###.##%;\-###.##%;0%"/>
+    <numFmt numFmtId="178" formatCode="&quot;—&quot;"/>
+    <numFmt numFmtId="179" formatCode="###%;###%;0%"/>
+    <numFmt numFmtId="180" formatCode="#,##0;\-#,###;0"/>
     <numFmt numFmtId="181" formatCode="#,##0.##;\-#,##0.##;0"/>
     <numFmt numFmtId="182" formatCode="#,###;#,###;0"/>
   </numFmts>
@@ -463,9 +456,6 @@
     <xf numFmtId="178" fontId="12" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="12" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,6 +466,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="12" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -590,7 +583,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F6FF-42D0-A8DC-6DDAB932C94F}"/>
+              <c16:uniqueId val="{00000000-3587-458C-A2A3-E51D5F6C5007}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -654,7 +647,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F6FF-42D0-A8DC-6DDAB932C94F}"/>
+              <c16:uniqueId val="{00000001-3587-458C-A2A3-E51D5F6C5007}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -718,7 +711,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F6FF-42D0-A8DC-6DDAB932C94F}"/>
+              <c16:uniqueId val="{00000002-3587-458C-A2A3-E51D5F6C5007}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -776,7 +769,7 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="0"/>
+              <c:idx val="1"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -831,9 +824,6 @@
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-F6FF-42D0-A8DC-6DDAB932C94F}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -939,7 +929,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-F6FF-42D0-A8DC-6DDAB932C94F}"/>
+              <c16:uniqueId val="{00000004-3587-458C-A2A3-E51D5F6C5007}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1249,7 +1239,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1DC4-48CE-BA2C-A64FCA7680BE}"/>
+              <c16:uniqueId val="{00000000-73C1-4980-87C6-2028049BB47B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1313,7 +1303,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1DC4-48CE-BA2C-A64FCA7680BE}"/>
+              <c16:uniqueId val="{00000001-73C1-4980-87C6-2028049BB47B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1377,7 +1367,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1DC4-48CE-BA2C-A64FCA7680BE}"/>
+              <c16:uniqueId val="{00000002-73C1-4980-87C6-2028049BB47B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1435,7 +1425,7 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="0"/>
+              <c:idx val="1"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1490,9 +1480,6 @@
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-1DC4-48CE-BA2C-A64FCA7680BE}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1598,7 +1585,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-1DC4-48CE-BA2C-A64FCA7680BE}"/>
+              <c16:uniqueId val="{00000004-73C1-4980-87C6-2028049BB47B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1956,7 +1943,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D55C-47F9-81EE-72044BE2F548}"/>
+              <c16:uniqueId val="{00000000-C8DF-4AD7-B654-209896CC8E39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2068,7 +2055,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D55C-47F9-81EE-72044BE2F548}"/>
+              <c16:uniqueId val="{00000001-C8DF-4AD7-B654-209896CC8E39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2180,7 +2167,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D55C-47F9-81EE-72044BE2F548}"/>
+              <c16:uniqueId val="{00000002-C8DF-4AD7-B654-209896CC8E39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2238,7 +2225,7 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="0"/>
+              <c:idx val="9"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -2293,9 +2280,6 @@
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-D55C-47F9-81EE-72044BE2F548}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2449,7 +2433,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D55C-47F9-81EE-72044BE2F548}"/>
+              <c16:uniqueId val="{00000004-C8DF-4AD7-B654-209896CC8E39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2777,7 +2761,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D246-46AE-B8CE-9030D8E64E8B}"/>
+              <c16:uniqueId val="{00000000-A6FA-47FE-96E0-DA72F8E437AF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2859,7 +2843,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D246-46AE-B8CE-9030D8E64E8B}"/>
+              <c16:uniqueId val="{00000001-A6FA-47FE-96E0-DA72F8E437AF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2941,7 +2925,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D246-46AE-B8CE-9030D8E64E8B}"/>
+              <c16:uniqueId val="{00000002-A6FA-47FE-96E0-DA72F8E437AF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2999,7 +2983,7 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="0"/>
+              <c:idx val="4"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -3054,9 +3038,6 @@
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-D246-46AE-B8CE-9030D8E64E8B}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3180,7 +3161,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D246-46AE-B8CE-9030D8E64E8B}"/>
+              <c16:uniqueId val="{00000004-A6FA-47FE-96E0-DA72F8E437AF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3508,7 +3489,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-44EF-45DA-869E-8EE092B9D355}"/>
+              <c16:uniqueId val="{00000000-837D-43F8-B56C-97C6350F07F6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3590,7 +3571,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-44EF-45DA-869E-8EE092B9D355}"/>
+              <c16:uniqueId val="{00000001-837D-43F8-B56C-97C6350F07F6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3672,7 +3653,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-44EF-45DA-869E-8EE092B9D355}"/>
+              <c16:uniqueId val="{00000002-837D-43F8-B56C-97C6350F07F6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3730,7 +3711,7 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="0"/>
+              <c:idx val="4"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -3785,9 +3766,6 @@
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-44EF-45DA-869E-8EE092B9D355}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3911,7 +3889,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-44EF-45DA-869E-8EE092B9D355}"/>
+              <c16:uniqueId val="{00000004-837D-43F8-B56C-97C6350F07F6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4215,7 +4193,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9BBB-41E0-AC8F-6EB417F87FAF}"/>
+              <c16:uniqueId val="{00000000-43E1-4CE9-BCBB-A539FF0F3488}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4273,7 +4251,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9BBB-41E0-AC8F-6EB417F87FAF}"/>
+              <c16:uniqueId val="{00000001-43E1-4CE9-BCBB-A539FF0F3488}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4331,7 +4309,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9BBB-41E0-AC8F-6EB417F87FAF}"/>
+              <c16:uniqueId val="{00000002-43E1-4CE9-BCBB-A539FF0F3488}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4446,7 +4424,7 @@
                   </c15:spPr>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-9BBB-41E0-AC8F-6EB417F87FAF}"/>
+                  <c16:uniqueId val="{00000003-43E1-4CE9-BCBB-A539FF0F3488}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -4546,7 +4524,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-9BBB-41E0-AC8F-6EB417F87FAF}"/>
+              <c16:uniqueId val="{00000004-43E1-4CE9-BCBB-A539FF0F3488}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4850,7 +4828,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FD1B-4DF4-92D4-1FEE6A315DE2}"/>
+              <c16:uniqueId val="{00000000-24C5-4ECC-8E3A-98721E86E0FD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4908,7 +4886,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FD1B-4DF4-92D4-1FEE6A315DE2}"/>
+              <c16:uniqueId val="{00000001-24C5-4ECC-8E3A-98721E86E0FD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4966,7 +4944,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FD1B-4DF4-92D4-1FEE6A315DE2}"/>
+              <c16:uniqueId val="{00000002-24C5-4ECC-8E3A-98721E86E0FD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5081,7 +5059,7 @@
                   </c15:spPr>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-FD1B-4DF4-92D4-1FEE6A315DE2}"/>
+                  <c16:uniqueId val="{00000003-24C5-4ECC-8E3A-98721E86E0FD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -5181,7 +5159,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-FD1B-4DF4-92D4-1FEE6A315DE2}"/>
+              <c16:uniqueId val="{00000004-24C5-4ECC-8E3A-98721E86E0FD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5410,7 +5388,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AD3EE29-FE57-408F-8157-E6D9A99C235F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D935C44-9ACA-4852-BBBB-08BD24B0538E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5443,7 +5421,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{313A3275-4300-4C04-8CF8-9F9A36A6E0A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47D2EB72-393C-400D-B700-27AE8407812E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5476,7 +5454,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1558A2D2-3783-4804-B585-BC169F689EE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30D7D55A-BEAB-476D-92E2-C530DBF705E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5509,7 +5487,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C61866B-C1C9-4231-96E8-9422BF463ADF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2BC067A-E404-403A-90BB-7849563D7AD1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5542,7 +5520,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F420FAA0-D55D-47F5-BAC0-E248AE3AC71A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{628DFFE8-3007-4C91-9A8A-A5F6CB67DCAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5575,7 +5553,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D586F25C-98CF-476D-9BD7-452922345740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D521EE2-DB24-44A6-ACB4-61517CC3B88C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5608,7 +5586,7 @@
         <xdr:cNvPr id="2" name="圖表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9470972D-7CD3-463C-B931-09FC8DEB27E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3CED6BD-B9C7-4432-875F-049DC9357B0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6032,31 +6010,31 @@
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="C3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="16">
         <v>1</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="12" t="s">
+      <c r="G3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6067,31 +6045,31 @@
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="12">
+      <c r="C4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="16">
         <v>1</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="16" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6102,31 +6080,31 @@
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="16">
         <v>3</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="16">
         <v>2</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="16">
         <v>4</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="16">
         <v>5</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="16">
         <v>5</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="16">
         <v>5</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="16">
         <v>5</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="16">
         <v>5</v>
       </c>
     </row>
@@ -6137,31 +6115,31 @@
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="12">
+      <c r="C6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="16">
         <v>2</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="16">
         <v>4</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="16">
         <v>1</v>
       </c>
-      <c r="J6" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="12">
+      <c r="J6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="16">
         <v>3</v>
       </c>
     </row>
@@ -6170,33 +6148,33 @@
         <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="12">
+        <v>46</v>
+      </c>
+      <c r="C7" s="16">
         <v>1</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="16">
         <v>3</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="16">
         <v>2</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="16">
         <v>2.5</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="16">
         <v>3.5</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="16">
         <v>4.5</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="16">
         <v>3</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="16">
         <v>3</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="16">
         <v>4</v>
       </c>
     </row>
@@ -6207,31 +6185,31 @@
       <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="12">
+      <c r="C8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="16">
         <v>3</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="12">
+      <c r="H8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="16">
         <v>2</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="16">
         <v>4</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="16">
         <v>1</v>
       </c>
     </row>
@@ -6242,31 +6220,31 @@
       <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="12" t="s">
+      <c r="C9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="16" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6275,33 +6253,33 @@
         <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="12">
+        <v>47</v>
+      </c>
+      <c r="C10" s="16">
         <v>1</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="16">
         <v>3</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="16">
         <v>2</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="16">
         <v>2.5</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="16">
         <v>3.38</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="16">
         <v>4.5</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="16">
         <v>2.75</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="16">
         <v>3.25</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="16">
         <v>3.25</v>
       </c>
     </row>
@@ -6312,31 +6290,31 @@
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" s="12" t="s">
+      <c r="C11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="16" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6347,51 +6325,51 @@
       <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="16">
         <v>1</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="16">
         <v>3</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="16">
         <v>2</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="16">
         <v>2.5</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="16">
         <v>3.38</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="16">
         <v>4.5</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="16">
         <v>2.75</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="16">
         <v>3.25</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="16">
         <v>3.25</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" location="'1.1.1.1 學士班繁星推薦入學錄取率'!A1" display="學士班繁星推薦入學錄取率" xr:uid="{B9AF61CE-82D8-4381-AD4E-C796A90FBAE4}"/>
-    <hyperlink ref="B4" location="'1.1.3.4 博士班招收國內重點大學畢業生比率'!A1" display="博士班招收國內重點大學畢業生比率" xr:uid="{6A3CC4BC-D2EB-4E98-951D-F575FA42F728}"/>
-    <hyperlink ref="B5" location="'1.4.1.1 學士班獲獎助學金平均金額'!A1" display="學士班獲獎助學金平均金額" xr:uid="{F2A05493-B27D-4F1E-B764-AA84E46A7D29}"/>
-    <hyperlink ref="B6" location="'1.7.1.4 碩士班平均修業年限'!A1" display="碩士班平均修業年限" xr:uid="{6E0C6988-5947-4C8B-B580-95B8D8B1B410}"/>
-    <hyperlink ref="B8" location="'2.1.1.2 平均碩博士班修課學生人數'!A1" display="平均碩博士班修課學生人數" xr:uid="{83A5CC13-1E14-4D1E-B506-A5F03909F49D}"/>
-    <hyperlink ref="B9" location="'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!A1" display="各系所教師兼任本校二級學術行政主管人次" xr:uid="{A8285FA1-BB51-43A6-9661-C5D920F89214}"/>
-    <hyperlink ref="B11" location="'3.2.1.1 舉辦國際學術研討會數'!A1" display="舉辦國際學術研討會數" xr:uid="{58B16260-07ED-4125-B8FF-B441EBB2AB43}"/>
+    <hyperlink ref="B3" location="'1.1.1.1 學士班繁星推薦入學錄取率'!A1" display="學士班繁星推薦入學錄取率" xr:uid="{BFCF7DC1-5619-4E5A-9487-F12CB1B2E480}"/>
+    <hyperlink ref="B4" location="'1.1.3.4 博士班招收國內重點大學畢業生比率'!A1" display="博士班招收國內重點大學畢業生比率" xr:uid="{94F34ED9-1A73-4CA2-B2C3-AC5C1298BF88}"/>
+    <hyperlink ref="B5" location="'1.4.1.1 學士班獲獎助學金平均金額'!A1" display="學士班獲獎助學金平均金額" xr:uid="{0E3156B6-EA92-448D-9794-078A2B45EF35}"/>
+    <hyperlink ref="B6" location="'1.7.1.4 碩士班平均修業年限'!A1" display="碩士班平均修業年限" xr:uid="{B0BCACE2-5E4B-4FD9-8705-CF0D9D3AF63A}"/>
+    <hyperlink ref="B8" location="'2.1.1.2 平均碩博士班修課學生人數'!A1" display="平均碩博士班修課學生人數" xr:uid="{08BE6B94-4454-4936-A493-5C1D98E6E95A}"/>
+    <hyperlink ref="B9" location="'2.3.1.2 各系所教師兼任本校二級學術行政主管人次'!A1" display="各系所教師兼任本校二級學術行政主管人次" xr:uid="{9D4F4DB3-0DAF-4B38-94B5-615817F23BD7}"/>
+    <hyperlink ref="B11" location="'3.2.1.1 舉辦國際學術研討會數'!A1" display="舉辦國際學術研討會數" xr:uid="{91E93907-9084-4ED3-B487-3DC94E819DE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFE835D-5FA1-42F6-BD7E-C5890EC438C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A8B7DD-68A1-43FF-ACDC-54E74B7671E7}">
   <sheetPr codeName="工作表1" filterMode="1"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -6403,8 +6381,7 @@
   <cols>
     <col min="1" max="1" width="40.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="12" style="6" customWidth="1"/>
-    <col min="3" max="3" width="6.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="7.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="7.25" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="6"/>
     <col min="9" max="9" width="14" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
@@ -6433,7 +6410,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
@@ -6443,16 +6420,16 @@
       <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="10">
         <v>0.20300000000000001</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="10">
         <v>0.17560000000000001</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="10">
         <v>0.23230000000000001</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="10">
         <v>0.20930000000000001</v>
       </c>
       <c r="G2" s="9">
@@ -6466,16 +6443,16 @@
       <c r="B3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="10">
         <v>0.20300000000000001</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="10">
         <v>0.17560000000000001</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="10">
         <v>0.23230000000000001</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>0.20930000000000001</v>
       </c>
       <c r="G3" s="9">
@@ -6489,16 +6466,16 @@
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="C4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -6512,16 +6489,16 @@
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="C5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -6535,16 +6512,16 @@
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="C6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="9" t="s">
@@ -6558,16 +6535,16 @@
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="C7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -6581,16 +6558,16 @@
       <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -6604,16 +6581,16 @@
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="C9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -6627,16 +6604,16 @@
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -6650,16 +6627,16 @@
       <c r="B11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="C11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -6677,7 +6654,7 @@
       <sortCondition ref="G1:G11"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G3">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
     <sortCondition ref="G2"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6688,7 +6665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB05E8DE-675A-4806-BB56-D1E5BCBFEC77}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EBED4B-E3FC-45EC-9316-0EB62307D62C}">
   <sheetPr codeName="工作表2" filterMode="1"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -6700,8 +6677,7 @@
   <cols>
     <col min="1" max="1" width="40.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="12" style="6" customWidth="1"/>
-    <col min="3" max="4" width="7.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="7.25" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="6"/>
     <col min="9" max="9" width="14" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
@@ -6730,7 +6706,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
@@ -6740,16 +6716,16 @@
       <c r="B2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="10">
         <v>0.47620000000000001</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="10">
         <v>0.66669999999999996</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="12">
         <v>0.8</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="12">
         <v>0.2</v>
       </c>
       <c r="G2" s="9">
@@ -6763,16 +6739,16 @@
       <c r="B3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="10">
         <v>0.47620000000000001</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="10">
         <v>0.66669999999999996</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="12">
         <v>0.8</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="12">
         <v>0.2</v>
       </c>
       <c r="G3" s="9">
@@ -6786,16 +6762,16 @@
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="C4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -6809,16 +6785,16 @@
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="C5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -6832,16 +6808,16 @@
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="C6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="9" t="s">
@@ -6855,16 +6831,16 @@
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="C7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -6878,16 +6854,16 @@
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -6901,16 +6877,16 @@
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="C9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -6924,16 +6900,16 @@
       <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -6947,16 +6923,16 @@
       <c r="B11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="C11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -6974,7 +6950,7 @@
       <sortCondition ref="G1:G11"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G3">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
     <sortCondition ref="G2"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6985,7 +6961,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A2EB8F-FE70-4B3E-B7AF-DB605DE823BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A3315B-160A-4BE0-B948-CA16B1B63D3B}">
   <sheetPr codeName="工作表3" filterMode="1"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -6997,7 +6973,7 @@
   <cols>
     <col min="1" max="1" width="40.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="12" style="6" customWidth="1"/>
-    <col min="3" max="6" width="6.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.5" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="6"/>
     <col min="9" max="9" width="14" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
@@ -7026,7 +7002,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
@@ -7036,16 +7012,16 @@
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="13">
         <v>53772.83</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="13">
         <v>50456.26</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="13">
         <v>64744.5</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="13">
         <v>47782</v>
       </c>
       <c r="G2" s="9">
@@ -7059,16 +7035,16 @@
       <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="13">
         <v>41252.32</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="13">
         <v>46152.42</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="13">
         <v>41276.49</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="13">
         <v>35494</v>
       </c>
       <c r="G3" s="9">
@@ -7082,16 +7058,16 @@
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="13">
         <v>40073.550000000003</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="13">
         <v>43548.23</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="13">
         <v>41720.04</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="13">
         <v>34551</v>
       </c>
       <c r="G4" s="9">
@@ -7105,16 +7081,16 @@
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="13">
         <v>38931.15</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="13">
         <v>32597.69</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="13">
         <v>39759.24</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="13">
         <v>45437</v>
       </c>
       <c r="G5" s="9">
@@ -7128,16 +7104,16 @@
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="13">
         <v>0</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="D6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="9">
@@ -7151,16 +7127,16 @@
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="13">
         <v>0</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="9">
@@ -7174,16 +7150,16 @@
       <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="13">
         <v>0</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="9">
@@ -7197,16 +7173,16 @@
       <c r="B9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="13">
         <v>0</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="D9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="9">
@@ -7220,16 +7196,16 @@
       <c r="B10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="13">
         <v>0</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="9">
@@ -7243,16 +7219,16 @@
       <c r="B11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="13">
         <v>42887.73</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="13">
         <v>43904.04</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="13">
         <v>45562.89</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="13">
         <v>39264.29</v>
       </c>
       <c r="G11" s="9">
@@ -7281,7 +7257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19F5E22-D916-4BCD-97D0-02E18B1014A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0F026B-83E6-4329-AFE0-63D472F2E113}">
   <sheetPr codeName="工作表4" filterMode="1"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -7293,8 +7269,7 @@
   <cols>
     <col min="1" max="1" width="40.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="12" style="6" customWidth="1"/>
-    <col min="3" max="5" width="4.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.25" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="6"/>
     <col min="9" max="9" width="14" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
@@ -7323,7 +7298,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
@@ -7333,16 +7308,16 @@
       <c r="B2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>2.56</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>2.5</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="15">
         <v>3</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>2.5</v>
       </c>
       <c r="G2" s="9">
@@ -7356,16 +7331,16 @@
       <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>3.02</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>3</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>2.93</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>3.2</v>
       </c>
       <c r="G3" s="9">
@@ -7379,16 +7354,16 @@
       <c r="B4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>3.48</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>3.32</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>3.44</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>3.7</v>
       </c>
       <c r="G4" s="9">
@@ -7402,16 +7377,16 @@
       <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>4.6100000000000003</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>4.8600000000000003</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>4.6100000000000003</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>4.3</v>
       </c>
       <c r="G5" s="9">
@@ -7425,16 +7400,16 @@
       <c r="B6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>3.52</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>3.43</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>3.64</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>3.5</v>
       </c>
       <c r="G6" s="9">
@@ -7448,16 +7423,16 @@
       <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="C7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -7471,16 +7446,16 @@
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -7494,16 +7469,16 @@
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="C9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -7517,16 +7492,16 @@
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -7540,16 +7515,16 @@
       <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="C11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -7567,7 +7542,7 @@
       <sortCondition ref="G1:G11"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
     <sortCondition ref="G2"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7578,7 +7553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0023B561-3B19-406F-941B-6AA8C8489125}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A661767-1CEF-4C56-A1BB-3626BFC6BA23}">
   <sheetPr codeName="工作表5" filterMode="1"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -7590,7 +7565,8 @@
   <cols>
     <col min="1" max="1" width="40.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="12" style="6" customWidth="1"/>
-    <col min="3" max="6" width="5.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.25" style="6" customWidth="1"/>
+    <col min="4" max="6" width="9.25" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="6"/>
     <col min="9" max="9" width="14" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
@@ -7619,7 +7595,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
@@ -7629,16 +7605,16 @@
       <c r="B2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>14.54</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>15.48</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>13.44</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>14.95</v>
       </c>
       <c r="G2" s="9">
@@ -7652,16 +7628,16 @@
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>12.56</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>14</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>13.67</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>10.27</v>
       </c>
       <c r="G3" s="9">
@@ -7675,16 +7651,16 @@
       <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>12.17</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>11.74</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>11.78</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>13.06</v>
       </c>
       <c r="G4" s="9">
@@ -7698,16 +7674,16 @@
       <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>3.67</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>2.4300000000000002</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>4.42</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>4.25</v>
       </c>
       <c r="G5" s="9">
@@ -7721,16 +7697,16 @@
       <c r="B6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>15.4</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>15.85</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>15.12</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>15.29</v>
       </c>
       <c r="G6" s="9">
@@ -7744,16 +7720,16 @@
       <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="C7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -7767,16 +7743,16 @@
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -7790,16 +7766,16 @@
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="C9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -7813,16 +7789,16 @@
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -7836,16 +7812,16 @@
       <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="C11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -7863,7 +7839,7 @@
       <sortCondition ref="G1:G11"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
     <sortCondition ref="G2"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7874,7 +7850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42746D9E-8FA0-4D8B-A85D-86186C1EB401}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED4DBEE-597A-4EB0-B1C6-8972A51ECE4B}">
   <sheetPr codeName="工作表6" filterMode="1"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -7886,7 +7862,7 @@
   <cols>
     <col min="1" max="1" width="40.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="12" style="6" customWidth="1"/>
-    <col min="3" max="6" width="3.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.25" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="6"/>
     <col min="9" max="9" width="14" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
@@ -7915,7 +7891,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
@@ -7925,16 +7901,16 @@
       <c r="B2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <v>2</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <v>1</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="15">
         <v>2</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="15">
         <v>3</v>
       </c>
       <c r="G2" s="9">
@@ -7948,16 +7924,16 @@
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="C3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G3" s="9" t="s">
@@ -7971,16 +7947,16 @@
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="C4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -7994,16 +7970,16 @@
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="C5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -8017,16 +7993,16 @@
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="C6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="9" t="s">
@@ -8040,16 +8016,16 @@
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="C7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -8063,16 +8039,16 @@
       <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -8086,16 +8062,16 @@
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="C9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -8109,16 +8085,16 @@
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -8132,16 +8108,16 @@
       <c r="B11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="C11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -8159,7 +8135,7 @@
       <sortCondition ref="G1:G11"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G2">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
     <sortCondition ref="G2"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -8170,7 +8146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D7E4C7-E6B3-4004-858B-736003CB1B69}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACAB0B6-1C96-4DE6-B7F5-B539961D7553}">
   <sheetPr codeName="工作表7" filterMode="1"/>
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -8211,7 +8187,7 @@
         <v>40</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
@@ -8221,16 +8197,16 @@
       <c r="B2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="C2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="9">
@@ -8244,16 +8220,16 @@
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="C3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G3" s="9" t="s">
@@ -8267,16 +8243,16 @@
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="C4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -8290,16 +8266,16 @@
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="C5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -8313,16 +8289,16 @@
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="C6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="9" t="s">
@@ -8336,16 +8312,16 @@
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="C7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -8359,16 +8335,16 @@
       <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -8382,16 +8358,16 @@
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="C9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -8405,16 +8381,16 @@
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -8428,16 +8404,16 @@
       <c r="B11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="C11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -8455,7 +8431,7 @@
       <sortCondition ref="G1:G11"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G2">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
     <sortCondition ref="G2"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>